<commit_message>
Remove unneeded iw-flex-gap mixin hack
</commit_message>
<xml_diff>
--- a/brad/Used components.xlsx
+++ b/brad/Used components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darek\Documents\Working\workspace\iw-components\brad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B785681-FE17-4654-BA02-18C2E3589C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6978B8E-CA46-46DE-9C53-CFE4EBA626DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58017E3D-A62E-4F28-8AB8-6076C1B7B7D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58017E3D-A62E-4F28-8AB8-6076C1B7B7D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -55,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="94">
   <si>
     <t>Transitions projects</t>
   </si>
@@ -341,9 +335,6 @@
   </si>
   <si>
     <t>* { box-sizing: border-box; }</t>
-  </si>
-  <si>
-    <t>iw-flex-gap(…) mixin hack</t>
   </si>
   <si>
     <t>progress</t>
@@ -454,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -466,16 +457,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,7 +469,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -507,11 +488,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -523,19 +499,18 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -544,13 +519,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -869,7 +844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -877,71 +852,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8035C7-2429-4AEE-B555-0DBC3EC2A1FF}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="31"/>
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="B1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="14" t="s">
+    <row r="2" spans="1:14" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="3"/>
@@ -949,9 +924,9 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -959,43 +934,43 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="3"/>
@@ -1003,31 +978,31 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="15" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="3"/>
@@ -1035,33 +1010,33 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="17" t="s">
         <v>86</v>
       </c>
       <c r="K6" s="3"/>
@@ -1069,21 +1044,21 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="27" t="s">
+      <c r="C7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="3"/>
@@ -1095,9 +1070,9 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1121,9 +1096,9 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1147,9 +1122,9 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1176,9 +1151,9 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="16" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1188,7 +1163,7 @@
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="20" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="3"/>
@@ -1200,9 +1175,9 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1220,7 +1195,7 @@
       <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -1234,721 +1209,687 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="16" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="16" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
-      <c r="B16" s="16" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="F16" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="16" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8" t="s">
+      <c r="F20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="8"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8" t="s">
+      <c r="F22" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J22" s="8"/>
+      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="F24" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="34"/>
-      <c r="B25" s="16" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8" t="s">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="8"/>
+      <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="34"/>
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="8"/>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
-      <c r="B29" s="16" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="16" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="8" t="s">
+      <c r="J30" s="3" t="s">
         <v>79</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
-      <c r="B32" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="8"/>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
-      <c r="B34" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
+      <c r="B34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
-      <c r="B35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="29"/>
+      <c r="B35" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
-      <c r="B36" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="29"/>
+      <c r="B36" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
-      <c r="B37" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="12" t="s">
-        <v>9</v>
-      </c>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="29"/>
+      <c r="B37" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="37"/>
-      <c r="B38" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="29"/>
+      <c r="B38" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="9"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="37"/>
-      <c r="B39" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
-      <c r="B40" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
+      <c r="B40" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="37"/>
-      <c r="B41" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="30"/>
+      <c r="B41" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="38"/>
-      <c r="B42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1958,8 +1899,8 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="A19:A32"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="A19:A31"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>

</xml_diff>